<commit_message>
Update Test case documents - ldbach
</commit_message>
<xml_diff>
--- a/doc/Project Assignment/PA05/TestCase_Group04.xlsx
+++ b/doc/Project Assignment/PA05/TestCase_Group04.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duy-Bach\Desktop\Git\cs300-assignment1\doc\Project Assignment\PA05\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="1"/>
   </bookViews>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="129">
   <si>
     <t>ID</t>
   </si>
@@ -439,11 +444,48 @@
   <si>
     <t>Sharing</t>
   </si>
+  <si>
+    <t>Function 07: Progress Tracking</t>
+  </si>
+  <si>
+    <t>S-PT-01</t>
+  </si>
+  <si>
+    <t>User click "See achievements" button, cahnge layout to Achivement View</t>
+  </si>
+  <si>
+    <t>User click "See pet's desire" button, cahnge layout to Achivement View</t>
+  </si>
+  <si>
+    <t>1. Currently in DiaryScene
+2. Click "See achievements" button</t>
+  </si>
+  <si>
+    <t>1. Currently in DiaryScene
+2. Click "See achievements" button
+3. Wait for Achievement screen come up
+4. Click "See Pet's Desire" button</t>
+  </si>
+  <si>
+    <t>The layout change to Achievement view</t>
+  </si>
+  <si>
+    <t>The layout change to Achievement view, and turn back to Quest View after clicking "See Pet's Desire" button</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>LDBach</t>
+  </si>
+  <si>
+    <t>17/12/207</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -475,7 +517,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -492,11 +534,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -514,6 +567,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,7 +709,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -686,9 +742,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -721,6 +794,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -996,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1739,24 +1829,76 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="3"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="3"/>
+      <c r="A29" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>105</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>